<commit_message>
new test case added
</commit_message>
<xml_diff>
--- a/OnlineBankingSystem/Test Data/Customers.xlsx
+++ b/OnlineBankingSystem/Test Data/Customers.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAIR\Desktop\MrRealProject\OnlineBankingSystem\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F87D6BE-97A3-4822-A291-A1589FA3E036}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C02CB634-D50C-4886-A285-0F8BF245A598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{A6BDE6BE-9D1E-460D-B22D-A3D72C21BCB5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="5895" xr2:uid="{A6BDE6BE-9D1E-460D-B22D-A3D72C21BCB5}"/>
   </bookViews>
   <sheets>
     <sheet name="CustData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -112,9 +108,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,10 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +459,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,8 +533,8 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2">
-        <v>36809</v>
+      <c r="F2" s="3">
+        <v>36961</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>

</xml_diff>